<commit_message>
crear ver, editar y eliminar productos
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\source\repos\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4534EAAA-00DE-4560-BA99-24376F65F8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D600620-7B27-4DA8-BD7C-71FEF2B006DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -212,6 +212,42 @@
   </si>
   <si>
     <t>Ver el menu de admin</t>
+  </si>
+  <si>
+    <t>Caso #13</t>
+  </si>
+  <si>
+    <t>Crear Producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear Producto </t>
+  </si>
+  <si>
+    <t>Caso #14</t>
+  </si>
+  <si>
+    <t>Ver Productos</t>
+  </si>
+  <si>
+    <t>Ver lista de productos</t>
+  </si>
+  <si>
+    <t>Caso #15</t>
+  </si>
+  <si>
+    <t>Caso #16</t>
+  </si>
+  <si>
+    <t>Editar porducto</t>
+  </si>
+  <si>
+    <t>Editar producto (solo admin)</t>
+  </si>
+  <si>
+    <t>Borrar porducto</t>
+  </si>
+  <si>
+    <t>Borrar producto (solo admin)</t>
   </si>
 </sst>
 </file>
@@ -310,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -340,8 +376,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1011,40 +1047,96 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
+      <c r="A19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
+      <c r="A20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
+      <c r="A21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
+      <c r="A22" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>

</xml_diff>

<commit_message>
crear, ver, editar y eliminar reseña admin
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\source\repos\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D600620-7B27-4DA8-BD7C-71FEF2B006DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AE7E59-6322-4DFF-89FC-F29786F34E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -248,6 +248,27 @@
   </si>
   <si>
     <t>Borrar producto (solo admin)</t>
+  </si>
+  <si>
+    <t>Caso #17</t>
+  </si>
+  <si>
+    <t>Caso #18</t>
+  </si>
+  <si>
+    <t>Caso #19</t>
+  </si>
+  <si>
+    <t>Ver reseña (admin)</t>
+  </si>
+  <si>
+    <t>Editar reseña</t>
+  </si>
+  <si>
+    <t>Eliminar reseña</t>
+  </si>
+  <si>
+    <t>Ver reseña desde el menu de admin</t>
   </si>
 </sst>
 </file>
@@ -595,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1139,31 +1160,73 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
+      <c r="A23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
+      <c r="A24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>

</xml_diff>

<commit_message>
agregado ingreso de compras y vista de compras PF, fin día 14-12
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AE7E59-6322-4DFF-89FC-F29786F34E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F074BA3-D3C2-411D-92DD-71F1FE55F1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -269,6 +269,33 @@
   </si>
   <si>
     <t>Ver reseña desde el menu de admin</t>
+  </si>
+  <si>
+    <t>Caso #20</t>
+  </si>
+  <si>
+    <t>Caso #21</t>
+  </si>
+  <si>
+    <t>Caso #22</t>
+  </si>
+  <si>
+    <t>Ingresar compra</t>
+  </si>
+  <si>
+    <t>Ver compras usuario</t>
+  </si>
+  <si>
+    <t>Ver compras admin</t>
+  </si>
+  <si>
+    <t>Ingrersar compra desde menu de usuario</t>
+  </si>
+  <si>
+    <t>Ver compras hechas por el usuario logueado</t>
+  </si>
+  <si>
+    <t>Ver las compras de todos los usuarios</t>
   </si>
 </sst>
 </file>
@@ -617,7 +644,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:G25"/>
+      <selection activeCell="E26" sqref="E26:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1229,31 +1256,73 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
+      <c r="A26" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
+      <c r="A27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
+      <c r="A28" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>

</xml_diff>

<commit_message>
reescritas funciones sin ClassBasedView y agregado avatar, fin día 15
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F074BA3-D3C2-411D-92DD-71F1FE55F1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBA4235-9893-45F1-A237-46D93C2CE7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Registrar usuario</t>
   </si>
   <si>
-    <t>Lograr registrar un usuario desde un forms propio, verificándolo desde el panel de admin</t>
-  </si>
-  <si>
     <t>Caso #9</t>
   </si>
   <si>
@@ -181,12 +178,6 @@
     <t>Hacer un logout</t>
   </si>
   <si>
-    <t>Lograr hacer login</t>
-  </si>
-  <si>
-    <t>Lograr hacer logout</t>
-  </si>
-  <si>
     <t>Login requerido?</t>
   </si>
   <si>
@@ -220,33 +211,21 @@
     <t>Crear Producto</t>
   </si>
   <si>
-    <t xml:space="preserve">Crear Producto </t>
-  </si>
-  <si>
     <t>Caso #14</t>
   </si>
   <si>
     <t>Ver Productos</t>
   </si>
   <si>
-    <t>Ver lista de productos</t>
-  </si>
-  <si>
     <t>Caso #15</t>
   </si>
   <si>
     <t>Caso #16</t>
   </si>
   <si>
-    <t>Editar porducto</t>
-  </si>
-  <si>
     <t>Editar producto (solo admin)</t>
   </si>
   <si>
-    <t>Borrar porducto</t>
-  </si>
-  <si>
     <t>Borrar producto (solo admin)</t>
   </si>
   <si>
@@ -296,6 +275,81 @@
   </si>
   <si>
     <t>Ver las compras de todos los usuarios</t>
+  </si>
+  <si>
+    <t>Caso #23</t>
+  </si>
+  <si>
+    <t>Caso #24</t>
+  </si>
+  <si>
+    <t>Ver Perfil</t>
+  </si>
+  <si>
+    <t>Editar Perfil</t>
+  </si>
+  <si>
+    <t>Ver perfil activo</t>
+  </si>
+  <si>
+    <t>Editar perfil activo</t>
+  </si>
+  <si>
+    <t>Editar producto</t>
+  </si>
+  <si>
+    <t>Ver lista de productos (admin)</t>
+  </si>
+  <si>
+    <t>Editar reseña (solo admin)</t>
+  </si>
+  <si>
+    <t>Eliminar reseña (solo admin)</t>
+  </si>
+  <si>
+    <t>Borrar producto</t>
+  </si>
+  <si>
+    <t>Crear reseña</t>
+  </si>
+  <si>
+    <t>Crear Producto, no se debe poder si el modelo ya existe (solo admin).</t>
+  </si>
+  <si>
+    <t>Crear reseña, no se debe poder si el modelo ya existe (solo admin).</t>
+  </si>
+  <si>
+    <t>Crear o editar avatar</t>
+  </si>
+  <si>
+    <t>Crear o editar avatar desde menu de usuario o admin</t>
+  </si>
+  <si>
+    <t>Caso #25</t>
+  </si>
+  <si>
+    <t>Caso #26</t>
+  </si>
+  <si>
+    <t>Lograr hacer login, ver página de login correcto.</t>
+  </si>
+  <si>
+    <t>Lograr hacer logout, ver página de logout correcto.</t>
+  </si>
+  <si>
+    <t>Lograr registrar un usuario desde un forms propio, , ver página de registro correcto.</t>
+  </si>
+  <si>
+    <t>Caso #27</t>
+  </si>
+  <si>
+    <t>Ver avatar</t>
+  </si>
+  <si>
+    <t>Se debe ver el avatar en todas las p{aginas del proyecto</t>
+  </si>
+  <si>
+    <t>Hasta el momento se ven, falta hacer la parte de blog</t>
   </si>
 </sst>
 </file>
@@ -641,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:G28"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -733,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>19</v>
@@ -756,7 +810,7 @@
         <v>45271</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>26</v>
@@ -798,7 +852,7 @@
         <v>45271</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>26</v>
@@ -840,7 +894,7 @@
         <v>45271</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>26</v>
@@ -882,7 +936,7 @@
         <v>45271</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>32</v>
@@ -905,7 +959,7 @@
         <v>45271</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>37</v>
@@ -947,7 +1001,7 @@
         <v>45272</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>41</v>
@@ -970,7 +1024,7 @@
         <v>45272</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>26</v>
@@ -987,13 +1041,13 @@
         <v>47</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="D14" s="7">
-        <v>45273</v>
+        <v>45275</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>26</v>
@@ -1004,19 +1058,19 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="7">
+        <v>45275</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" s="7">
-        <v>45273</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>26</v>
@@ -1027,19 +1081,19 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="D16" s="7">
-        <v>45273</v>
+        <v>45275</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>26</v>
@@ -1050,19 +1104,19 @@
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D17" s="7">
         <v>45273</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>26</v>
@@ -1073,19 +1127,19 @@
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="D18" s="7">
         <v>45273</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>26</v>
@@ -1096,19 +1150,19 @@
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="D19" s="7">
         <v>45274</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>26</v>
@@ -1119,19 +1173,19 @@
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D20" s="7">
         <v>45274</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>26</v>
@@ -1142,19 +1196,19 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D21" s="7">
         <v>45274</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>26</v>
@@ -1165,19 +1219,19 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D22" s="7">
         <v>45274</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>26</v>
@@ -1188,19 +1242,19 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="D23" s="7">
         <v>45274</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>26</v>
@@ -1211,19 +1265,19 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D24" s="7">
         <v>45274</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>26</v>
@@ -1234,19 +1288,19 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D25" s="7">
         <v>45274</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>26</v>
@@ -1257,19 +1311,19 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D26" s="7">
         <v>45274</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>26</v>
@@ -1280,19 +1334,19 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D27" s="7">
         <v>45274</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>26</v>
@@ -1303,19 +1357,19 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D28" s="7">
         <v>45274</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>26</v>
@@ -1325,49 +1379,119 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
+      <c r="A29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="7">
+        <v>45274</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="13"/>
+      <c r="A30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="7">
+        <v>45275</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
+      <c r="A31" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="7">
+        <v>45275</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="13"/>
+      <c r="A32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="7">
+        <v>45275</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
+      <c r="A33" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="7">
+        <v>45275</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
@@ -1504,22 +1628,30 @@
       <c r="F48" s="12"/>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2456,6 +2588,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
crear blog y editar blog
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBA4235-9893-45F1-A237-46D93C2CE7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A2B2D-AA9A-458D-B238-F8E867DCA9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="116">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -350,6 +350,24 @@
   </si>
   <si>
     <t>Hasta el momento se ven, falta hacer la parte de blog</t>
+  </si>
+  <si>
+    <t>Caso #28</t>
+  </si>
+  <si>
+    <t>Crear Blog</t>
+  </si>
+  <si>
+    <t>Crear Blog desde el menu propio de admin</t>
+  </si>
+  <si>
+    <t>Caso #29</t>
+  </si>
+  <si>
+    <t>Ver listado de blogs (admin)</t>
+  </si>
+  <si>
+    <t>Ver listado de Blogs desde el menu propio de admin</t>
   </si>
 </sst>
 </file>
@@ -698,7 +716,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="E35" sqref="E35:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -894,7 +912,7 @@
         <v>45271</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>26</v>
@@ -936,7 +954,7 @@
         <v>45271</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>32</v>
@@ -1001,7 +1019,7 @@
         <v>45272</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>41</v>
@@ -1093,7 +1111,7 @@
         <v>45275</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>26</v>
@@ -1494,22 +1512,50 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="13"/>
+      <c r="A34" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="7">
+        <v>45276</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="13"/>
+      <c r="A35" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="7">
+        <v>45276</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>

</xml_diff>

<commit_message>
crear, ver, editar y eliminar posts
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690A2B2D-AA9A-458D-B238-F8E867DCA9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AE1B4C-5B77-432C-97DF-83C07C6A00A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="128">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -368,6 +368,42 @@
   </si>
   <si>
     <t>Ver listado de Blogs desde el menu propio de admin</t>
+  </si>
+  <si>
+    <t>Ver listado de blogs (user)</t>
+  </si>
+  <si>
+    <t>Eliminar blog</t>
+  </si>
+  <si>
+    <t>Ver listado de blogs desde el link de home</t>
+  </si>
+  <si>
+    <t>Ver detalle de blog (admin)</t>
+  </si>
+  <si>
+    <t>Ver detalle de blog (user)</t>
+  </si>
+  <si>
+    <t>Ver delalle de blog desde el menu propio de admin</t>
+  </si>
+  <si>
+    <t>Ver delalle de blog desde el listado que ve el user</t>
+  </si>
+  <si>
+    <t>Eliminar Blog desde el menu propio de admin</t>
+  </si>
+  <si>
+    <t>Caso #30</t>
+  </si>
+  <si>
+    <t>Caso #31</t>
+  </si>
+  <si>
+    <t>Caso #32</t>
+  </si>
+  <si>
+    <t>Caso #33</t>
   </si>
 </sst>
 </file>
@@ -716,7 +752,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35:G35"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1558,40 +1594,96 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="13"/>
+      <c r="A36" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="7">
+        <v>45277</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="13"/>
+      <c r="A37" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="7">
+        <v>45277</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="13"/>
+      <c r="A38" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="7">
+        <v>45277</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="13"/>
+      <c r="A39" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="7">
+        <v>45277</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>

</xml_diff>

<commit_message>
finalizado PF, se modificará si se encuentran errores
</commit_message>
<xml_diff>
--- a/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
+++ b/Proyecto_final_Salerno/pruebas/pruebas en desarrollo/Casos de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\código\mi_code\Proyecto_final_Salerno\pruebas\pruebas en desarrollo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AE1B4C-5B77-432C-97DF-83C07C6A00A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9922A4D-EF5E-49EF-9E34-70D0B516F3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="134">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>120.0.6099.71</t>
-  </si>
-  <si>
     <t>Bruno Salerno</t>
   </si>
   <si>
@@ -404,6 +401,27 @@
   </si>
   <si>
     <t>Caso #33</t>
+  </si>
+  <si>
+    <t>Ver comentarios</t>
+  </si>
+  <si>
+    <t>Comentar</t>
+  </si>
+  <si>
+    <t>Ver comentarios de cada post</t>
+  </si>
+  <si>
+    <t>Comentar en un post determinado</t>
+  </si>
+  <si>
+    <t>Caso #34</t>
+  </si>
+  <si>
+    <t>Caso #35</t>
+  </si>
+  <si>
+    <t>120.0.6099.110</t>
   </si>
 </sst>
 </file>
@@ -752,7 +770,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -783,14 +801,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="B2" s="2">
+        <v>35</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
+      <c r="D2" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -799,13 +819,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="15"/>
     </row>
@@ -814,13 +834,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="15"/>
     </row>
@@ -832,19 +852,19 @@
         <v>7</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>9</v>
@@ -855,22 +875,22 @@
         <v>10</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="7">
         <v>45271</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
@@ -897,22 +917,22 @@
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="7">
         <v>45271</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -939,22 +959,22 @@
         <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="7">
         <v>45271</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -978,48 +998,48 @@
     </row>
     <row r="10" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>30</v>
-      </c>
       <c r="C10" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="7">
         <v>45271</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="D11" s="7">
         <v>45271</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -1043,665 +1063,693 @@
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="7">
         <v>45272</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>44</v>
       </c>
       <c r="D13" s="7">
         <v>45272</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="C14" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="7">
         <v>45275</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" s="7">
         <v>45275</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="7">
         <v>45275</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="D17" s="7">
         <v>45273</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="D18" s="7">
         <v>45273</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="C19" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="7">
         <v>45274</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="C20" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" s="7">
         <v>45274</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="7">
         <v>45274</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" s="7">
         <v>45274</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="7">
         <v>45274</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="7">
         <v>45274</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D25" s="7">
         <v>45274</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="7">
         <v>45274</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="7">
         <v>45274</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="7">
         <v>45274</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" s="7">
         <v>45274</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="C30" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="7">
         <v>45275</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="7">
         <v>45275</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="D32" s="7">
         <v>45275</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>107</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="D33" s="7">
         <v>45275</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D34" s="7">
         <v>45276</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>115</v>
       </c>
       <c r="D35" s="7">
         <v>45276</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D36" s="7">
         <v>45277</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D37" s="7">
         <v>45277</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D38" s="7">
         <v>45277</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D39" s="7">
         <v>45277</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
+      <c r="A40" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="7">
+        <v>45277</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="13"/>
+      <c r="A41" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="7">
+        <v>45277</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>

</xml_diff>